<commit_message>
Insert patchbays into drawings
</commit_message>
<xml_diff>
--- a/Patch Bays.xlsx
+++ b/Patch Bays.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="17565" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="17565"/>
   </bookViews>
   <sheets>
     <sheet name="HD SDI" sheetId="1" r:id="rId1"/>
     <sheet name="Audio" sheetId="9" r:id="rId2"/>
+    <sheet name="Misc" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>JF A</t>
   </si>
@@ -61,9 +62,6 @@
     <t>REF</t>
   </si>
   <si>
-    <t>JF F</t>
-  </si>
-  <si>
     <t>I/P 01</t>
   </si>
   <si>
@@ -143,6 +141,9 @@
   </si>
   <si>
     <t>Coms A</t>
+  </si>
+  <si>
+    <t>Cam Power</t>
   </si>
 </sst>
 </file>
@@ -219,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,8 +257,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -289,11 +296,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,37 +377,43 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -672,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,42 +776,42 @@
       <c r="S1" s="14"/>
       <c r="T1" s="14"/>
       <c r="U1" s="14"/>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="17" t="s">
         <v>7</v>
       </c>
       <c r="X1" s="10"/>
     </row>
     <row r="2" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17" t="s">
+      <c r="I2" s="22"/>
+      <c r="J2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="18"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="15"/>
       <c r="M2" s="13"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="19" t="s">
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="16" t="s">
         <v>12</v>
       </c>
       <c r="X2" s="10"/>
-      <c r="Z2" s="15" t="s">
+      <c r="Z2" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -771,7 +821,7 @@
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="X3" s="8"/>
-      <c r="Z3" s="15"/>
+      <c r="Z3" s="23"/>
     </row>
     <row r="4" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -842,7 +892,7 @@
       <c r="X4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="Z4" s="15"/>
+      <c r="Z4" s="23"/>
     </row>
     <row r="5" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -885,38 +935,38 @@
       <c r="X6" s="10"/>
     </row>
     <row r="7" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
       <c r="M7" s="13"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
       <c r="V7" s="13"/>
       <c r="X7" s="10"/>
-      <c r="Z7" s="15" t="s">
+      <c r="Z7" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="X8" s="8"/>
-      <c r="Z8" s="15"/>
+      <c r="Z8" s="23"/>
     </row>
     <row r="9" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -987,7 +1037,7 @@
       <c r="X9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="Z9" s="15"/>
+      <c r="Z9" s="23"/>
     </row>
     <row r="10" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1012,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,89 +1140,105 @@
     </row>
     <row r="2" spans="1:22" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="T2" s="8"/>
-      <c r="V2" s="16" t="s">
+      <c r="V2" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="E3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="F3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="G3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="H3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="J3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="K3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="L3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="M3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="N3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="O3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="25" t="s">
+      <c r="P3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="Q3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="25" t="s">
+      <c r="R3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="25" t="s">
+      <c r="T3" s="10"/>
+      <c r="V3" s="24"/>
+    </row>
+    <row r="4" spans="1:22" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="10"/>
-      <c r="V3" s="16"/>
-    </row>
-    <row r="4" spans="1:22" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="25" t="s">
+      <c r="D4" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
       <c r="T4" s="10"/>
-      <c r="V4" s="16"/>
+      <c r="V4" s="24"/>
     </row>
     <row r="5" spans="1:22" s="11" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="T5" s="8"/>
-      <c r="V5" s="16"/>
+      <c r="V5" s="24"/>
     </row>
     <row r="6" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1231,200 +1297,132 @@
       <c r="T6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="V6" s="21"/>
-    </row>
-    <row r="7" spans="1:22" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="V6" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="V2:V5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" style="1" customWidth="1"/>
+    <col min="3" max="18" width="11.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" style="7" customWidth="1"/>
+    <col min="21" max="21" width="2.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="5.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="10"/>
+      <c r="V1" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T2" s="8"/>
+      <c r="V2" s="24"/>
+    </row>
+    <row r="3" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4">
+      <c r="B3" s="2"/>
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F3" s="4">
         <v>4</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G3" s="4">
         <v>5</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H3" s="4">
         <v>6</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I3" s="4">
         <v>7</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J3" s="4">
         <v>8</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K3" s="4">
         <v>9</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L3" s="4">
         <v>10</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M3" s="4">
         <v>11</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N3" s="4">
         <v>12</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O3" s="4">
         <v>13</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P3" s="4">
         <v>14</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q3" s="4">
         <v>15</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R3" s="4">
         <v>16</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="6" t="s">
+      <c r="S3" s="3"/>
+      <c r="T3" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T9" s="8"/>
-      <c r="V9" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="R10" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="T10" s="10"/>
-      <c r="V10" s="16"/>
-    </row>
-    <row r="11" spans="1:22" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="T11" s="10"/>
-      <c r="V11" s="16"/>
-    </row>
-    <row r="12" spans="1:22" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T12" s="8"/>
-      <c r="V12" s="16"/>
-    </row>
-    <row r="13" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4">
-        <v>3</v>
-      </c>
-      <c r="F13" s="4">
-        <v>4</v>
-      </c>
-      <c r="G13" s="4">
-        <v>5</v>
-      </c>
-      <c r="H13" s="4">
-        <v>6</v>
-      </c>
-      <c r="I13" s="4">
-        <v>7</v>
-      </c>
-      <c r="J13" s="4">
-        <v>8</v>
-      </c>
-      <c r="K13" s="4">
-        <v>9</v>
-      </c>
-      <c r="L13" s="4">
-        <v>10</v>
-      </c>
-      <c r="M13" s="4">
-        <v>11</v>
-      </c>
-      <c r="N13" s="4">
-        <v>12</v>
-      </c>
-      <c r="O13" s="4">
-        <v>13</v>
-      </c>
-      <c r="P13" s="4">
-        <v>14</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>15</v>
-      </c>
-      <c r="R13" s="4">
-        <v>16</v>
-      </c>
-      <c r="S13" s="3"/>
-      <c r="T13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" s="21"/>
+      <c r="V3" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="V2:V5"/>
-    <mergeCell ref="V9:V12"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
RTR O/P to JF
</commit_message>
<xml_diff>
--- a/Patch Bays.xlsx
+++ b/Patch Bays.xlsx
@@ -453,10 +453,19 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,15 +478,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -868,17 +868,17 @@
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="24"/>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="35"/>
-      <c r="M2" s="36"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="32"/>
       <c r="N2" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="29"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
       <c r="T2" s="15"/>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="2" spans="1:22" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="T2" s="8"/>
-      <c r="V2" s="30" t="s">
+      <c r="V2" s="33" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
         <v>28</v>
       </c>
       <c r="T3" s="10"/>
-      <c r="V3" s="30"/>
+      <c r="V3" s="33"/>
     </row>
     <row r="4" spans="1:22" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="21" t="s">
@@ -1311,11 +1311,11 @@
         <v>38</v>
       </c>
       <c r="T4" s="10"/>
-      <c r="V4" s="30"/>
+      <c r="V4" s="33"/>
     </row>
     <row r="5" spans="1:22" s="11" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="T5" s="8"/>
-      <c r="V5" s="30"/>
+      <c r="V5" s="33"/>
     </row>
     <row r="6" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
@@ -1411,12 +1411,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
@@ -1438,13 +1438,13 @@
         <v>43</v>
       </c>
       <c r="T1" s="10"/>
-      <c r="V1" s="30" t="s">
+      <c r="V1" s="33" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="T2" s="8"/>
-      <c r="V2" s="30"/>
+      <c r="V2" s="33"/>
     </row>
     <row r="3" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
@@ -1503,7 +1503,7 @@
       <c r="T3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="30"/>
+      <c r="V3" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Re-arrange coms on patchbay
</commit_message>
<xml_diff>
--- a/Patch Bays.xlsx
+++ b/Patch Bays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="3300" windowWidth="28730" windowHeight="17570"/>
+    <workbookView xWindow="1940" yWindow="3300" windowWidth="28730" windowHeight="17570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HD SDI" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>JF A</t>
   </si>
@@ -786,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,26 +1416,30 @@
       </c>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="19"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="20" t="s">
+      <c r="K1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="R1" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="Q1" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="20" t="s">
-        <v>43</v>
       </c>
       <c r="T1" s="10"/>
       <c r="V1" s="33" t="s">
@@ -1508,7 +1512,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="V1:V3"/>
-    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape"/>

</xml_diff>